<commit_message>
Updated Merge Lead paage and find merge lead page
</commit_message>
<xml_diff>
--- a/data/TC007.xlsx
+++ b/data/TC007.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>crmsfa</t>
+  </si>
+  <si>
+    <t>leaf</t>
+  </si>
+  <si>
+    <t>Indhu</t>
   </si>
 </sst>
 </file>
@@ -75,12 +81,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +394,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,11 +426,11 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>10047</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10049</v>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>